<commit_message>
Sidebar icons are finished
</commit_message>
<xml_diff>
--- a/Список_дел.xlsx
+++ b/Список_дел.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">Номер</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">Сделать иконки для сайдбара</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Не совсем</t>
   </si>
   <si>
     <t xml:space="preserve">Страница с инструкцией</t>
@@ -181,10 +178,10 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.31"/>
@@ -238,7 +235,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -246,7 +243,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -255,7 +252,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -264,7 +261,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3"/>
     </row>

</xml_diff>